<commit_message>
POC Test Case completed
</commit_message>
<xml_diff>
--- a/testData/air_marketing_testData.xlsx
+++ b/testData/air_marketing_testData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
   </bookViews>
   <sheets>
     <sheet name="testRunner" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="58">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -23,9 +23,6 @@
     <t>UK</t>
   </si>
   <si>
-    <t>POC Test Case</t>
-  </si>
-  <si>
     <t>YES</t>
   </si>
   <si>
@@ -38,9 +35,6 @@
     <t>Test Case 01</t>
   </si>
   <si>
-    <t>Test Case 02</t>
-  </si>
-  <si>
     <t>Test Case 03</t>
   </si>
   <si>
@@ -68,18 +62,6 @@
     <t>NO</t>
   </si>
   <si>
-    <t>POC Test Data Key 01</t>
-  </si>
-  <si>
-    <t>POC Test Data Key 02</t>
-  </si>
-  <si>
-    <t>POC Test Data Value 01</t>
-  </si>
-  <si>
-    <t>POC Test Data Value 02</t>
-  </si>
-  <si>
     <t>POC Test Data Key 03</t>
   </si>
   <si>
@@ -186,6 +168,27 @@
   </si>
   <si>
     <t>TC1 Test Data Value 10</t>
+  </si>
+  <si>
+    <t>POC_TC01_GrabLockIssue</t>
+  </si>
+  <si>
+    <t>Campaign</t>
+  </si>
+  <si>
+    <t>Liv'd</t>
+  </si>
+  <si>
+    <t>Data List</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Livd-Manufacturing </t>
+  </si>
+  <si>
+    <t>Sample Test Case 01</t>
+  </si>
+  <si>
+    <t>Sample Test Case 02</t>
   </si>
 </sst>
 </file>
@@ -237,28 +240,27 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="7">
     <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="9" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -286,56 +288,24 @@
         </patternFill>
       </fill>
     </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <condense val="0"/>
-        <extend val="0"/>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" mergeCell="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
 </styleSheet>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="testRunner" displayName="testRunner" ref="A1:B12" totalsRowShown="0" headerRowDxfId="6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="testRunner" displayName="testRunner" ref="A1:B12" totalsRowShown="0" headerRowDxfId="3">
   <tableColumns count="2">
     <tableColumn id="1" name="Test Case Name"/>
-    <tableColumn id="2" name="UK" dataDxfId="7"/>
+    <tableColumn id="2" name="UK" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium9" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="testData" displayName="testData" ref="A1:C21" totalsRowShown="0" headerRowDxfId="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="testData" displayName="testData" ref="A1:C21" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:C21"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Test Case Name"/>
     <tableColumn id="2" name="Test Data Key"/>
@@ -632,7 +602,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
@@ -652,100 +622,103 @@
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>6</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="3" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>"NO"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
       <formula>"YES"</formula>
     </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A2:A12">
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B12">
@@ -764,8 +737,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:C21"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12:C21"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -779,178 +752,230 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>4</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>51</v>
       </c>
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C5" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="C6" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="B4" t="s">
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C7" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="B5" s="3" t="s">
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C8" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="B6" t="s">
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>51</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C9" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="B7" s="3" t="s">
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="B8" t="s">
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C11" t="s">
         <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
-      <c r="B9" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="B10" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
-      <c r="B11" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:3">
       <c r="A12" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B15" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C15" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3" t="s">
+    <row r="16" spans="1:3">
+      <c r="A16" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C16" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
-      <c r="B14" s="3" t="s">
+    <row r="17" spans="1:3">
+      <c r="A17" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B17" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
-      <c r="B15" s="3" t="s">
+    <row r="18" spans="1:3">
+      <c r="A18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C18" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="B16" s="3" t="s">
+    <row r="19" spans="1:3">
+      <c r="A19" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="3" t="s">
+    <row r="20" spans="1:3">
+      <c r="A20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="3" t="s">
+    <row r="21" spans="1:3">
+      <c r="A21" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C21" t="s">
         <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="C20" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>